<commit_message>
PROS-14717 LionJP Adjacency KPI release into production
</commit_message>
<xml_diff>
--- a/Projects/LIONJP/Data/kpi_template.xlsx
+++ b/Projects/LIONJP/Data/kpi_template.xlsx
@@ -5,25 +5,26 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="kpi_config_bak" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="kpi_config" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="kpi_config" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="kpi_config_test" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$1:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$1:$O$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config!$A$1:$O$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">kpi_config_test!$A$1:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">kpi_config_test!$A$2:$O$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="74">
   <si>
     <t xml:space="preserve">LionJP</t>
   </si>
@@ -254,6 +255,9 @@
   </si>
   <si>
     <t xml:space="preserve">4987643120059, 4987643121056, 4987643121063, 4987643122077, 4987643122084, 4987643122107, 4987643120066, 4987643122145, 4901301335678, 4901301337870, 4901301348975, 4901301351333, 4901301361721, 4901301382016, 4901301382023, 4901301382030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ver</t>
   </si>
 </sst>
 </file>
@@ -378,7 +382,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -408,6 +412,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,6 +495,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -490,15 +506,14 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,7 +864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -896,7 +911,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -943,7 +958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -990,7 +1005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1178,7 +1193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1272,7 +1287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1319,7 +1334,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1366,7 +1381,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1413,7 +1428,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1460,7 +1475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -1507,7 +1522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -1554,7 +1569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
@@ -1601,7 +1616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -1646,7 +1661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1692,16 +1707,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O26"/>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1710,31 +1727,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ26"/>
+  <dimension ref="1:35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="3:26"/>
+      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="44.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="42.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="6" width="106.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="21.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="6" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="6" width="10.65"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="6" width="103.80612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="6" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="6" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,13 +2834,13 @@
         <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>40</v>
@@ -2844,13 +2861,13 @@
         <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>26</v>
@@ -2858,1082 +2875,1307 @@
       <c r="O3" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
+      <c r="AJ3" s="0"/>
+      <c r="AK3" s="0"/>
+      <c r="AL3" s="0"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
+      <c r="AO3" s="0"/>
+      <c r="AP3" s="0"/>
+      <c r="AQ3" s="0"/>
+      <c r="AR3" s="0"/>
+      <c r="AS3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
+      <c r="AV3" s="0"/>
+      <c r="AW3" s="0"/>
+      <c r="AX3" s="0"/>
+      <c r="AY3" s="0"/>
+      <c r="AZ3" s="0"/>
+      <c r="BA3" s="0"/>
+      <c r="BB3" s="0"/>
+      <c r="BC3" s="0"/>
+      <c r="BD3" s="0"/>
+      <c r="BE3" s="0"/>
+      <c r="BF3" s="0"/>
+      <c r="BG3" s="0"/>
+      <c r="BH3" s="0"/>
+      <c r="BI3" s="0"/>
+      <c r="BJ3" s="0"/>
+      <c r="BK3" s="0"/>
+      <c r="BL3" s="0"/>
+      <c r="BM3" s="0"/>
+      <c r="BN3" s="0"/>
+      <c r="BO3" s="0"/>
+      <c r="BP3" s="0"/>
+      <c r="BQ3" s="0"/>
+      <c r="BR3" s="0"/>
+      <c r="BS3" s="0"/>
+      <c r="BT3" s="0"/>
+      <c r="BU3" s="0"/>
+      <c r="BV3" s="0"/>
+      <c r="BW3" s="0"/>
+      <c r="BX3" s="0"/>
+      <c r="BY3" s="0"/>
+      <c r="BZ3" s="0"/>
+      <c r="CA3" s="0"/>
+      <c r="CB3" s="0"/>
+      <c r="CC3" s="0"/>
+      <c r="CD3" s="0"/>
+      <c r="CE3" s="0"/>
+      <c r="CF3" s="0"/>
+      <c r="CG3" s="0"/>
+      <c r="CH3" s="0"/>
+      <c r="CI3" s="0"/>
+      <c r="CJ3" s="0"/>
+      <c r="CK3" s="0"/>
+      <c r="CL3" s="0"/>
+      <c r="CM3" s="0"/>
+      <c r="CN3" s="0"/>
+      <c r="CO3" s="0"/>
+      <c r="CP3" s="0"/>
+      <c r="CQ3" s="0"/>
+      <c r="CR3" s="0"/>
+      <c r="CS3" s="0"/>
+      <c r="CT3" s="0"/>
+      <c r="CU3" s="0"/>
+      <c r="CV3" s="0"/>
+      <c r="CW3" s="0"/>
+      <c r="CX3" s="0"/>
+      <c r="CY3" s="0"/>
+      <c r="CZ3" s="0"/>
+      <c r="DA3" s="0"/>
+      <c r="DB3" s="0"/>
+      <c r="DC3" s="0"/>
+      <c r="DD3" s="0"/>
+      <c r="DE3" s="0"/>
+      <c r="DF3" s="0"/>
+      <c r="DG3" s="0"/>
+      <c r="DH3" s="0"/>
+      <c r="DI3" s="0"/>
+      <c r="DJ3" s="0"/>
+      <c r="DK3" s="0"/>
+      <c r="DL3" s="0"/>
+      <c r="DM3" s="0"/>
+      <c r="DN3" s="0"/>
+      <c r="DO3" s="0"/>
+      <c r="DP3" s="0"/>
+      <c r="DQ3" s="0"/>
+      <c r="DR3" s="0"/>
+      <c r="DS3" s="0"/>
+      <c r="DT3" s="0"/>
+      <c r="DU3" s="0"/>
+      <c r="DV3" s="0"/>
+      <c r="DW3" s="0"/>
+      <c r="DX3" s="0"/>
+      <c r="DY3" s="0"/>
+      <c r="DZ3" s="0"/>
+      <c r="EA3" s="0"/>
+      <c r="EB3" s="0"/>
+      <c r="EC3" s="0"/>
+      <c r="ED3" s="0"/>
+      <c r="EE3" s="0"/>
+      <c r="EF3" s="0"/>
+      <c r="EG3" s="0"/>
+      <c r="EH3" s="0"/>
+      <c r="EI3" s="0"/>
+      <c r="EJ3" s="0"/>
+      <c r="EK3" s="0"/>
+      <c r="EL3" s="0"/>
+      <c r="EM3" s="0"/>
+      <c r="EN3" s="0"/>
+      <c r="EO3" s="0"/>
+      <c r="EP3" s="0"/>
+      <c r="EQ3" s="0"/>
+      <c r="ER3" s="0"/>
+      <c r="ES3" s="0"/>
+      <c r="ET3" s="0"/>
+      <c r="EU3" s="0"/>
+      <c r="EV3" s="0"/>
+      <c r="EW3" s="0"/>
+      <c r="EX3" s="0"/>
+      <c r="EY3" s="0"/>
+      <c r="EZ3" s="0"/>
+      <c r="FA3" s="0"/>
+      <c r="FB3" s="0"/>
+      <c r="FC3" s="0"/>
+      <c r="FD3" s="0"/>
+      <c r="FE3" s="0"/>
+      <c r="FF3" s="0"/>
+      <c r="FG3" s="0"/>
+      <c r="FH3" s="0"/>
+      <c r="FI3" s="0"/>
+      <c r="FJ3" s="0"/>
+      <c r="FK3" s="0"/>
+      <c r="FL3" s="0"/>
+      <c r="FM3" s="0"/>
+      <c r="FN3" s="0"/>
+      <c r="FO3" s="0"/>
+      <c r="FP3" s="0"/>
+      <c r="FQ3" s="0"/>
+      <c r="FR3" s="0"/>
+      <c r="FS3" s="0"/>
+      <c r="FT3" s="0"/>
+      <c r="FU3" s="0"/>
+      <c r="FV3" s="0"/>
+      <c r="FW3" s="0"/>
+      <c r="FX3" s="0"/>
+      <c r="FY3" s="0"/>
+      <c r="FZ3" s="0"/>
+      <c r="GA3" s="0"/>
+      <c r="GB3" s="0"/>
+      <c r="GC3" s="0"/>
+      <c r="GD3" s="0"/>
+      <c r="GE3" s="0"/>
+      <c r="GF3" s="0"/>
+      <c r="GG3" s="0"/>
+      <c r="GH3" s="0"/>
+      <c r="GI3" s="0"/>
+      <c r="GJ3" s="0"/>
+      <c r="GK3" s="0"/>
+      <c r="GL3" s="0"/>
+      <c r="GM3" s="0"/>
+      <c r="GN3" s="0"/>
+      <c r="GO3" s="0"/>
+      <c r="GP3" s="0"/>
+      <c r="GQ3" s="0"/>
+      <c r="GR3" s="0"/>
+      <c r="GS3" s="0"/>
+      <c r="GT3" s="0"/>
+      <c r="GU3" s="0"/>
+      <c r="GV3" s="0"/>
+      <c r="GW3" s="0"/>
+      <c r="GX3" s="0"/>
+      <c r="GY3" s="0"/>
+      <c r="GZ3" s="0"/>
+      <c r="HA3" s="0"/>
+      <c r="HB3" s="0"/>
+      <c r="HC3" s="0"/>
+      <c r="HD3" s="0"/>
+      <c r="HE3" s="0"/>
+      <c r="HF3" s="0"/>
+      <c r="HG3" s="0"/>
+      <c r="HH3" s="0"/>
+      <c r="HI3" s="0"/>
+      <c r="HJ3" s="0"/>
+      <c r="HK3" s="0"/>
+      <c r="HL3" s="0"/>
+      <c r="HM3" s="0"/>
+      <c r="HN3" s="0"/>
+      <c r="HO3" s="0"/>
+      <c r="HP3" s="0"/>
+      <c r="HQ3" s="0"/>
+      <c r="HR3" s="0"/>
+      <c r="HS3" s="0"/>
+      <c r="HT3" s="0"/>
+      <c r="HU3" s="0"/>
+      <c r="HV3" s="0"/>
+      <c r="HW3" s="0"/>
+      <c r="HX3" s="0"/>
+      <c r="HY3" s="0"/>
+      <c r="HZ3" s="0"/>
+      <c r="IA3" s="0"/>
+      <c r="IB3" s="0"/>
+      <c r="IC3" s="0"/>
+      <c r="ID3" s="0"/>
+      <c r="IE3" s="0"/>
+      <c r="IF3" s="0"/>
+      <c r="IG3" s="0"/>
+      <c r="IH3" s="0"/>
+      <c r="II3" s="0"/>
+      <c r="IJ3" s="0"/>
+      <c r="IK3" s="0"/>
+      <c r="IL3" s="0"/>
+      <c r="IM3" s="0"/>
+      <c r="IN3" s="0"/>
+      <c r="IO3" s="0"/>
+      <c r="IP3" s="0"/>
+      <c r="IQ3" s="0"/>
+      <c r="IR3" s="0"/>
+      <c r="IS3" s="0"/>
+      <c r="IT3" s="0"/>
+      <c r="IU3" s="0"/>
+      <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
+      <c r="IX3" s="0"/>
+      <c r="IY3" s="0"/>
+      <c r="IZ3" s="0"/>
+      <c r="JA3" s="0"/>
+      <c r="JB3" s="0"/>
+      <c r="JC3" s="0"/>
+      <c r="JD3" s="0"/>
+      <c r="JE3" s="0"/>
+      <c r="JF3" s="0"/>
+      <c r="JG3" s="0"/>
+      <c r="JH3" s="0"/>
+      <c r="JI3" s="0"/>
+      <c r="JJ3" s="0"/>
+      <c r="JK3" s="0"/>
+      <c r="JL3" s="0"/>
+      <c r="JM3" s="0"/>
+      <c r="JN3" s="0"/>
+      <c r="JO3" s="0"/>
+      <c r="JP3" s="0"/>
+      <c r="JQ3" s="0"/>
+      <c r="JR3" s="0"/>
+      <c r="JS3" s="0"/>
+      <c r="JT3" s="0"/>
+      <c r="JU3" s="0"/>
+      <c r="JV3" s="0"/>
+      <c r="JW3" s="0"/>
+      <c r="JX3" s="0"/>
+      <c r="JY3" s="0"/>
+      <c r="JZ3" s="0"/>
+      <c r="KA3" s="0"/>
+      <c r="KB3" s="0"/>
+      <c r="KC3" s="0"/>
+      <c r="KD3" s="0"/>
+      <c r="KE3" s="0"/>
+      <c r="KF3" s="0"/>
+      <c r="KG3" s="0"/>
+      <c r="KH3" s="0"/>
+      <c r="KI3" s="0"/>
+      <c r="KJ3" s="0"/>
+      <c r="KK3" s="0"/>
+      <c r="KL3" s="0"/>
+      <c r="KM3" s="0"/>
+      <c r="KN3" s="0"/>
+      <c r="KO3" s="0"/>
+      <c r="KP3" s="0"/>
+      <c r="KQ3" s="0"/>
+      <c r="KR3" s="0"/>
+      <c r="KS3" s="0"/>
+      <c r="KT3" s="0"/>
+      <c r="KU3" s="0"/>
+      <c r="KV3" s="0"/>
+      <c r="KW3" s="0"/>
+      <c r="KX3" s="0"/>
+      <c r="KY3" s="0"/>
+      <c r="KZ3" s="0"/>
+      <c r="LA3" s="0"/>
+      <c r="LB3" s="0"/>
+      <c r="LC3" s="0"/>
+      <c r="LD3" s="0"/>
+      <c r="LE3" s="0"/>
+      <c r="LF3" s="0"/>
+      <c r="LG3" s="0"/>
+      <c r="LH3" s="0"/>
+      <c r="LI3" s="0"/>
+      <c r="LJ3" s="0"/>
+      <c r="LK3" s="0"/>
+      <c r="LL3" s="0"/>
+      <c r="LM3" s="0"/>
+      <c r="LN3" s="0"/>
+      <c r="LO3" s="0"/>
+      <c r="LP3" s="0"/>
+      <c r="LQ3" s="0"/>
+      <c r="LR3" s="0"/>
+      <c r="LS3" s="0"/>
+      <c r="LT3" s="0"/>
+      <c r="LU3" s="0"/>
+      <c r="LV3" s="0"/>
+      <c r="LW3" s="0"/>
+      <c r="LX3" s="0"/>
+      <c r="LY3" s="0"/>
+      <c r="LZ3" s="0"/>
+      <c r="MA3" s="0"/>
+      <c r="MB3" s="0"/>
+      <c r="MC3" s="0"/>
+      <c r="MD3" s="0"/>
+      <c r="ME3" s="0"/>
+      <c r="MF3" s="0"/>
+      <c r="MG3" s="0"/>
+      <c r="MH3" s="0"/>
+      <c r="MI3" s="0"/>
+      <c r="MJ3" s="0"/>
+      <c r="MK3" s="0"/>
+      <c r="ML3" s="0"/>
+      <c r="MM3" s="0"/>
+      <c r="MN3" s="0"/>
+      <c r="MO3" s="0"/>
+      <c r="MP3" s="0"/>
+      <c r="MQ3" s="0"/>
+      <c r="MR3" s="0"/>
+      <c r="MS3" s="0"/>
+      <c r="MT3" s="0"/>
+      <c r="MU3" s="0"/>
+      <c r="MV3" s="0"/>
+      <c r="MW3" s="0"/>
+      <c r="MX3" s="0"/>
+      <c r="MY3" s="0"/>
+      <c r="MZ3" s="0"/>
+      <c r="NA3" s="0"/>
+      <c r="NB3" s="0"/>
+      <c r="NC3" s="0"/>
+      <c r="ND3" s="0"/>
+      <c r="NE3" s="0"/>
+      <c r="NF3" s="0"/>
+      <c r="NG3" s="0"/>
+      <c r="NH3" s="0"/>
+      <c r="NI3" s="0"/>
+      <c r="NJ3" s="0"/>
+      <c r="NK3" s="0"/>
+      <c r="NL3" s="0"/>
+      <c r="NM3" s="0"/>
+      <c r="NN3" s="0"/>
+      <c r="NO3" s="0"/>
+      <c r="NP3" s="0"/>
+      <c r="NQ3" s="0"/>
+      <c r="NR3" s="0"/>
+      <c r="NS3" s="0"/>
+      <c r="NT3" s="0"/>
+      <c r="NU3" s="0"/>
+      <c r="NV3" s="0"/>
+      <c r="NW3" s="0"/>
+      <c r="NX3" s="0"/>
+      <c r="NY3" s="0"/>
+      <c r="NZ3" s="0"/>
+      <c r="OA3" s="0"/>
+      <c r="OB3" s="0"/>
+      <c r="OC3" s="0"/>
+      <c r="OD3" s="0"/>
+      <c r="OE3" s="0"/>
+      <c r="OF3" s="0"/>
+      <c r="OG3" s="0"/>
+      <c r="OH3" s="0"/>
+      <c r="OI3" s="0"/>
+      <c r="OJ3" s="0"/>
+      <c r="OK3" s="0"/>
+      <c r="OL3" s="0"/>
+      <c r="OM3" s="0"/>
+      <c r="ON3" s="0"/>
+      <c r="OO3" s="0"/>
+      <c r="OP3" s="0"/>
+      <c r="OQ3" s="0"/>
+      <c r="OR3" s="0"/>
+      <c r="OS3" s="0"/>
+      <c r="OT3" s="0"/>
+      <c r="OU3" s="0"/>
+      <c r="OV3" s="0"/>
+      <c r="OW3" s="0"/>
+      <c r="OX3" s="0"/>
+      <c r="OY3" s="0"/>
+      <c r="OZ3" s="0"/>
+      <c r="PA3" s="0"/>
+      <c r="PB3" s="0"/>
+      <c r="PC3" s="0"/>
+      <c r="PD3" s="0"/>
+      <c r="PE3" s="0"/>
+      <c r="PF3" s="0"/>
+      <c r="PG3" s="0"/>
+      <c r="PH3" s="0"/>
+      <c r="PI3" s="0"/>
+      <c r="PJ3" s="0"/>
+      <c r="PK3" s="0"/>
+      <c r="PL3" s="0"/>
+      <c r="PM3" s="0"/>
+      <c r="PN3" s="0"/>
+      <c r="PO3" s="0"/>
+      <c r="PP3" s="0"/>
+      <c r="PQ3" s="0"/>
+      <c r="PR3" s="0"/>
+      <c r="PS3" s="0"/>
+      <c r="PT3" s="0"/>
+      <c r="PU3" s="0"/>
+      <c r="PV3" s="0"/>
+      <c r="PW3" s="0"/>
+      <c r="PX3" s="0"/>
+      <c r="PY3" s="0"/>
+      <c r="PZ3" s="0"/>
+      <c r="QA3" s="0"/>
+      <c r="QB3" s="0"/>
+      <c r="QC3" s="0"/>
+      <c r="QD3" s="0"/>
+      <c r="QE3" s="0"/>
+      <c r="QF3" s="0"/>
+      <c r="QG3" s="0"/>
+      <c r="QH3" s="0"/>
+      <c r="QI3" s="0"/>
+      <c r="QJ3" s="0"/>
+      <c r="QK3" s="0"/>
+      <c r="QL3" s="0"/>
+      <c r="QM3" s="0"/>
+      <c r="QN3" s="0"/>
+      <c r="QO3" s="0"/>
+      <c r="QP3" s="0"/>
+      <c r="QQ3" s="0"/>
+      <c r="QR3" s="0"/>
+      <c r="QS3" s="0"/>
+      <c r="QT3" s="0"/>
+      <c r="QU3" s="0"/>
+      <c r="QV3" s="0"/>
+      <c r="QW3" s="0"/>
+      <c r="QX3" s="0"/>
+      <c r="QY3" s="0"/>
+      <c r="QZ3" s="0"/>
+      <c r="RA3" s="0"/>
+      <c r="RB3" s="0"/>
+      <c r="RC3" s="0"/>
+      <c r="RD3" s="0"/>
+      <c r="RE3" s="0"/>
+      <c r="RF3" s="0"/>
+      <c r="RG3" s="0"/>
+      <c r="RH3" s="0"/>
+      <c r="RI3" s="0"/>
+      <c r="RJ3" s="0"/>
+      <c r="RK3" s="0"/>
+      <c r="RL3" s="0"/>
+      <c r="RM3" s="0"/>
+      <c r="RN3" s="0"/>
+      <c r="RO3" s="0"/>
+      <c r="RP3" s="0"/>
+      <c r="RQ3" s="0"/>
+      <c r="RR3" s="0"/>
+      <c r="RS3" s="0"/>
+      <c r="RT3" s="0"/>
+      <c r="RU3" s="0"/>
+      <c r="RV3" s="0"/>
+      <c r="RW3" s="0"/>
+      <c r="RX3" s="0"/>
+      <c r="RY3" s="0"/>
+      <c r="RZ3" s="0"/>
+      <c r="SA3" s="0"/>
+      <c r="SB3" s="0"/>
+      <c r="SC3" s="0"/>
+      <c r="SD3" s="0"/>
+      <c r="SE3" s="0"/>
+      <c r="SF3" s="0"/>
+      <c r="SG3" s="0"/>
+      <c r="SH3" s="0"/>
+      <c r="SI3" s="0"/>
+      <c r="SJ3" s="0"/>
+      <c r="SK3" s="0"/>
+      <c r="SL3" s="0"/>
+      <c r="SM3" s="0"/>
+      <c r="SN3" s="0"/>
+      <c r="SO3" s="0"/>
+      <c r="SP3" s="0"/>
+      <c r="SQ3" s="0"/>
+      <c r="SR3" s="0"/>
+      <c r="SS3" s="0"/>
+      <c r="ST3" s="0"/>
+      <c r="SU3" s="0"/>
+      <c r="SV3" s="0"/>
+      <c r="SW3" s="0"/>
+      <c r="SX3" s="0"/>
+      <c r="SY3" s="0"/>
+      <c r="SZ3" s="0"/>
+      <c r="TA3" s="0"/>
+      <c r="TB3" s="0"/>
+      <c r="TC3" s="0"/>
+      <c r="TD3" s="0"/>
+      <c r="TE3" s="0"/>
+      <c r="TF3" s="0"/>
+      <c r="TG3" s="0"/>
+      <c r="TH3" s="0"/>
+      <c r="TI3" s="0"/>
+      <c r="TJ3" s="0"/>
+      <c r="TK3" s="0"/>
+      <c r="TL3" s="0"/>
+      <c r="TM3" s="0"/>
+      <c r="TN3" s="0"/>
+      <c r="TO3" s="0"/>
+      <c r="TP3" s="0"/>
+      <c r="TQ3" s="0"/>
+      <c r="TR3" s="0"/>
+      <c r="TS3" s="0"/>
+      <c r="TT3" s="0"/>
+      <c r="TU3" s="0"/>
+      <c r="TV3" s="0"/>
+      <c r="TW3" s="0"/>
+      <c r="TX3" s="0"/>
+      <c r="TY3" s="0"/>
+      <c r="TZ3" s="0"/>
+      <c r="UA3" s="0"/>
+      <c r="UB3" s="0"/>
+      <c r="UC3" s="0"/>
+      <c r="UD3" s="0"/>
+      <c r="UE3" s="0"/>
+      <c r="UF3" s="0"/>
+      <c r="UG3" s="0"/>
+      <c r="UH3" s="0"/>
+      <c r="UI3" s="0"/>
+      <c r="UJ3" s="0"/>
+      <c r="UK3" s="0"/>
+      <c r="UL3" s="0"/>
+      <c r="UM3" s="0"/>
+      <c r="UN3" s="0"/>
+      <c r="UO3" s="0"/>
+      <c r="UP3" s="0"/>
+      <c r="UQ3" s="0"/>
+      <c r="UR3" s="0"/>
+      <c r="US3" s="0"/>
+      <c r="UT3" s="0"/>
+      <c r="UU3" s="0"/>
+      <c r="UV3" s="0"/>
+      <c r="UW3" s="0"/>
+      <c r="UX3" s="0"/>
+      <c r="UY3" s="0"/>
+      <c r="UZ3" s="0"/>
+      <c r="VA3" s="0"/>
+      <c r="VB3" s="0"/>
+      <c r="VC3" s="0"/>
+      <c r="VD3" s="0"/>
+      <c r="VE3" s="0"/>
+      <c r="VF3" s="0"/>
+      <c r="VG3" s="0"/>
+      <c r="VH3" s="0"/>
+      <c r="VI3" s="0"/>
+      <c r="VJ3" s="0"/>
+      <c r="VK3" s="0"/>
+      <c r="VL3" s="0"/>
+      <c r="VM3" s="0"/>
+      <c r="VN3" s="0"/>
+      <c r="VO3" s="0"/>
+      <c r="VP3" s="0"/>
+      <c r="VQ3" s="0"/>
+      <c r="VR3" s="0"/>
+      <c r="VS3" s="0"/>
+      <c r="VT3" s="0"/>
+      <c r="VU3" s="0"/>
+      <c r="VV3" s="0"/>
+      <c r="VW3" s="0"/>
+      <c r="VX3" s="0"/>
+      <c r="VY3" s="0"/>
+      <c r="VZ3" s="0"/>
+      <c r="WA3" s="0"/>
+      <c r="WB3" s="0"/>
+      <c r="WC3" s="0"/>
+      <c r="WD3" s="0"/>
+      <c r="WE3" s="0"/>
+      <c r="WF3" s="0"/>
+      <c r="WG3" s="0"/>
+      <c r="WH3" s="0"/>
+      <c r="WI3" s="0"/>
+      <c r="WJ3" s="0"/>
+      <c r="WK3" s="0"/>
+      <c r="WL3" s="0"/>
+      <c r="WM3" s="0"/>
+      <c r="WN3" s="0"/>
+      <c r="WO3" s="0"/>
+      <c r="WP3" s="0"/>
+      <c r="WQ3" s="0"/>
+      <c r="WR3" s="0"/>
+      <c r="WS3" s="0"/>
+      <c r="WT3" s="0"/>
+      <c r="WU3" s="0"/>
+      <c r="WV3" s="0"/>
+      <c r="WW3" s="0"/>
+      <c r="WX3" s="0"/>
+      <c r="WY3" s="0"/>
+      <c r="WZ3" s="0"/>
+      <c r="XA3" s="0"/>
+      <c r="XB3" s="0"/>
+      <c r="XC3" s="0"/>
+      <c r="XD3" s="0"/>
+      <c r="XE3" s="0"/>
+      <c r="XF3" s="0"/>
+      <c r="XG3" s="0"/>
+      <c r="XH3" s="0"/>
+      <c r="XI3" s="0"/>
+      <c r="XJ3" s="0"/>
+      <c r="XK3" s="0"/>
+      <c r="XL3" s="0"/>
+      <c r="XM3" s="0"/>
+      <c r="XN3" s="0"/>
+      <c r="XO3" s="0"/>
+      <c r="XP3" s="0"/>
+      <c r="XQ3" s="0"/>
+      <c r="XR3" s="0"/>
+      <c r="XS3" s="0"/>
+      <c r="XT3" s="0"/>
+      <c r="XU3" s="0"/>
+      <c r="XV3" s="0"/>
+      <c r="XW3" s="0"/>
+      <c r="XX3" s="0"/>
+      <c r="XY3" s="0"/>
+      <c r="XZ3" s="0"/>
+      <c r="YA3" s="0"/>
+      <c r="YB3" s="0"/>
+      <c r="YC3" s="0"/>
+      <c r="YD3" s="0"/>
+      <c r="YE3" s="0"/>
+      <c r="YF3" s="0"/>
+      <c r="YG3" s="0"/>
+      <c r="YH3" s="0"/>
+      <c r="YI3" s="0"/>
+      <c r="YJ3" s="0"/>
+      <c r="YK3" s="0"/>
+      <c r="YL3" s="0"/>
+      <c r="YM3" s="0"/>
+      <c r="YN3" s="0"/>
+      <c r="YO3" s="0"/>
+      <c r="YP3" s="0"/>
+      <c r="YQ3" s="0"/>
+      <c r="YR3" s="0"/>
+      <c r="YS3" s="0"/>
+      <c r="YT3" s="0"/>
+      <c r="YU3" s="0"/>
+      <c r="YV3" s="0"/>
+      <c r="YW3" s="0"/>
+      <c r="YX3" s="0"/>
+      <c r="YY3" s="0"/>
+      <c r="YZ3" s="0"/>
+      <c r="ZA3" s="0"/>
+      <c r="ZB3" s="0"/>
+      <c r="ZC3" s="0"/>
+      <c r="ZD3" s="0"/>
+      <c r="ZE3" s="0"/>
+      <c r="ZF3" s="0"/>
+      <c r="ZG3" s="0"/>
+      <c r="ZH3" s="0"/>
+      <c r="ZI3" s="0"/>
+      <c r="ZJ3" s="0"/>
+      <c r="ZK3" s="0"/>
+      <c r="ZL3" s="0"/>
+      <c r="ZM3" s="0"/>
+      <c r="ZN3" s="0"/>
+      <c r="ZO3" s="0"/>
+      <c r="ZP3" s="0"/>
+      <c r="ZQ3" s="0"/>
+      <c r="ZR3" s="0"/>
+      <c r="ZS3" s="0"/>
+      <c r="ZT3" s="0"/>
+      <c r="ZU3" s="0"/>
+      <c r="ZV3" s="0"/>
+      <c r="ZW3" s="0"/>
+      <c r="ZX3" s="0"/>
+      <c r="ZY3" s="0"/>
+      <c r="ZZ3" s="0"/>
+      <c r="AAA3" s="0"/>
+      <c r="AAB3" s="0"/>
+      <c r="AAC3" s="0"/>
+      <c r="AAD3" s="0"/>
+      <c r="AAE3" s="0"/>
+      <c r="AAF3" s="0"/>
+      <c r="AAG3" s="0"/>
+      <c r="AAH3" s="0"/>
+      <c r="AAI3" s="0"/>
+      <c r="AAJ3" s="0"/>
+      <c r="AAK3" s="0"/>
+      <c r="AAL3" s="0"/>
+      <c r="AAM3" s="0"/>
+      <c r="AAN3" s="0"/>
+      <c r="AAO3" s="0"/>
+      <c r="AAP3" s="0"/>
+      <c r="AAQ3" s="0"/>
+      <c r="AAR3" s="0"/>
+      <c r="AAS3" s="0"/>
+      <c r="AAT3" s="0"/>
+      <c r="AAU3" s="0"/>
+      <c r="AAV3" s="0"/>
+      <c r="AAW3" s="0"/>
+      <c r="AAX3" s="0"/>
+      <c r="AAY3" s="0"/>
+      <c r="AAZ3" s="0"/>
+      <c r="ABA3" s="0"/>
+      <c r="ABB3" s="0"/>
+      <c r="ABC3" s="0"/>
+      <c r="ABD3" s="0"/>
+      <c r="ABE3" s="0"/>
+      <c r="ABF3" s="0"/>
+      <c r="ABG3" s="0"/>
+      <c r="ABH3" s="0"/>
+      <c r="ABI3" s="0"/>
+      <c r="ABJ3" s="0"/>
+      <c r="ABK3" s="0"/>
+      <c r="ABL3" s="0"/>
+      <c r="ABM3" s="0"/>
+      <c r="ABN3" s="0"/>
+      <c r="ABO3" s="0"/>
+      <c r="ABP3" s="0"/>
+      <c r="ABQ3" s="0"/>
+      <c r="ABR3" s="0"/>
+      <c r="ABS3" s="0"/>
+      <c r="ABT3" s="0"/>
+      <c r="ABU3" s="0"/>
+      <c r="ABV3" s="0"/>
+      <c r="ABW3" s="0"/>
+      <c r="ABX3" s="0"/>
+      <c r="ABY3" s="0"/>
+      <c r="ABZ3" s="0"/>
+      <c r="ACA3" s="0"/>
+      <c r="ACB3" s="0"/>
+      <c r="ACC3" s="0"/>
+      <c r="ACD3" s="0"/>
+      <c r="ACE3" s="0"/>
+      <c r="ACF3" s="0"/>
+      <c r="ACG3" s="0"/>
+      <c r="ACH3" s="0"/>
+      <c r="ACI3" s="0"/>
+      <c r="ACJ3" s="0"/>
+      <c r="ACK3" s="0"/>
+      <c r="ACL3" s="0"/>
+      <c r="ACM3" s="0"/>
+      <c r="ACN3" s="0"/>
+      <c r="ACO3" s="0"/>
+      <c r="ACP3" s="0"/>
+      <c r="ACQ3" s="0"/>
+      <c r="ACR3" s="0"/>
+      <c r="ACS3" s="0"/>
+      <c r="ACT3" s="0"/>
+      <c r="ACU3" s="0"/>
+      <c r="ACV3" s="0"/>
+      <c r="ACW3" s="0"/>
+      <c r="ACX3" s="0"/>
+      <c r="ACY3" s="0"/>
+      <c r="ACZ3" s="0"/>
+      <c r="ADA3" s="0"/>
+      <c r="ADB3" s="0"/>
+      <c r="ADC3" s="0"/>
+      <c r="ADD3" s="0"/>
+      <c r="ADE3" s="0"/>
+      <c r="ADF3" s="0"/>
+      <c r="ADG3" s="0"/>
+      <c r="ADH3" s="0"/>
+      <c r="ADI3" s="0"/>
+      <c r="ADJ3" s="0"/>
+      <c r="ADK3" s="0"/>
+      <c r="ADL3" s="0"/>
+      <c r="ADM3" s="0"/>
+      <c r="ADN3" s="0"/>
+      <c r="ADO3" s="0"/>
+      <c r="ADP3" s="0"/>
+      <c r="ADQ3" s="0"/>
+      <c r="ADR3" s="0"/>
+      <c r="ADS3" s="0"/>
+      <c r="ADT3" s="0"/>
+      <c r="ADU3" s="0"/>
+      <c r="ADV3" s="0"/>
+      <c r="ADW3" s="0"/>
+      <c r="ADX3" s="0"/>
+      <c r="ADY3" s="0"/>
+      <c r="ADZ3" s="0"/>
+      <c r="AEA3" s="0"/>
+      <c r="AEB3" s="0"/>
+      <c r="AEC3" s="0"/>
+      <c r="AED3" s="0"/>
+      <c r="AEE3" s="0"/>
+      <c r="AEF3" s="0"/>
+      <c r="AEG3" s="0"/>
+      <c r="AEH3" s="0"/>
+      <c r="AEI3" s="0"/>
+      <c r="AEJ3" s="0"/>
+      <c r="AEK3" s="0"/>
+      <c r="AEL3" s="0"/>
+      <c r="AEM3" s="0"/>
+      <c r="AEN3" s="0"/>
+      <c r="AEO3" s="0"/>
+      <c r="AEP3" s="0"/>
+      <c r="AEQ3" s="0"/>
+      <c r="AER3" s="0"/>
+      <c r="AES3" s="0"/>
+      <c r="AET3" s="0"/>
+      <c r="AEU3" s="0"/>
+      <c r="AEV3" s="0"/>
+      <c r="AEW3" s="0"/>
+      <c r="AEX3" s="0"/>
+      <c r="AEY3" s="0"/>
+      <c r="AEZ3" s="0"/>
+      <c r="AFA3" s="0"/>
+      <c r="AFB3" s="0"/>
+      <c r="AFC3" s="0"/>
+      <c r="AFD3" s="0"/>
+      <c r="AFE3" s="0"/>
+      <c r="AFF3" s="0"/>
+      <c r="AFG3" s="0"/>
+      <c r="AFH3" s="0"/>
+      <c r="AFI3" s="0"/>
+      <c r="AFJ3" s="0"/>
+      <c r="AFK3" s="0"/>
+      <c r="AFL3" s="0"/>
+      <c r="AFM3" s="0"/>
+      <c r="AFN3" s="0"/>
+      <c r="AFO3" s="0"/>
+      <c r="AFP3" s="0"/>
+      <c r="AFQ3" s="0"/>
+      <c r="AFR3" s="0"/>
+      <c r="AFS3" s="0"/>
+      <c r="AFT3" s="0"/>
+      <c r="AFU3" s="0"/>
+      <c r="AFV3" s="0"/>
+      <c r="AFW3" s="0"/>
+      <c r="AFX3" s="0"/>
+      <c r="AFY3" s="0"/>
+      <c r="AFZ3" s="0"/>
+      <c r="AGA3" s="0"/>
+      <c r="AGB3" s="0"/>
+      <c r="AGC3" s="0"/>
+      <c r="AGD3" s="0"/>
+      <c r="AGE3" s="0"/>
+      <c r="AGF3" s="0"/>
+      <c r="AGG3" s="0"/>
+      <c r="AGH3" s="0"/>
+      <c r="AGI3" s="0"/>
+      <c r="AGJ3" s="0"/>
+      <c r="AGK3" s="0"/>
+      <c r="AGL3" s="0"/>
+      <c r="AGM3" s="0"/>
+      <c r="AGN3" s="0"/>
+      <c r="AGO3" s="0"/>
+      <c r="AGP3" s="0"/>
+      <c r="AGQ3" s="0"/>
+      <c r="AGR3" s="0"/>
+      <c r="AGS3" s="0"/>
+      <c r="AGT3" s="0"/>
+      <c r="AGU3" s="0"/>
+      <c r="AGV3" s="0"/>
+      <c r="AGW3" s="0"/>
+      <c r="AGX3" s="0"/>
+      <c r="AGY3" s="0"/>
+      <c r="AGZ3" s="0"/>
+      <c r="AHA3" s="0"/>
+      <c r="AHB3" s="0"/>
+      <c r="AHC3" s="0"/>
+      <c r="AHD3" s="0"/>
+      <c r="AHE3" s="0"/>
+      <c r="AHF3" s="0"/>
+      <c r="AHG3" s="0"/>
+      <c r="AHH3" s="0"/>
+      <c r="AHI3" s="0"/>
+      <c r="AHJ3" s="0"/>
+      <c r="AHK3" s="0"/>
+      <c r="AHL3" s="0"/>
+      <c r="AHM3" s="0"/>
+      <c r="AHN3" s="0"/>
+      <c r="AHO3" s="0"/>
+      <c r="AHP3" s="0"/>
+      <c r="AHQ3" s="0"/>
+      <c r="AHR3" s="0"/>
+      <c r="AHS3" s="0"/>
+      <c r="AHT3" s="0"/>
+      <c r="AHU3" s="0"/>
+      <c r="AHV3" s="0"/>
+      <c r="AHW3" s="0"/>
+      <c r="AHX3" s="0"/>
+      <c r="AHY3" s="0"/>
+      <c r="AHZ3" s="0"/>
+      <c r="AIA3" s="0"/>
+      <c r="AIB3" s="0"/>
+      <c r="AIC3" s="0"/>
+      <c r="AID3" s="0"/>
+      <c r="AIE3" s="0"/>
+      <c r="AIF3" s="0"/>
+      <c r="AIG3" s="0"/>
+      <c r="AIH3" s="0"/>
+      <c r="AII3" s="0"/>
+      <c r="AIJ3" s="0"/>
+      <c r="AIK3" s="0"/>
+      <c r="AIL3" s="0"/>
+      <c r="AIM3" s="0"/>
+      <c r="AIN3" s="0"/>
+      <c r="AIO3" s="0"/>
+      <c r="AIP3" s="0"/>
+      <c r="AIQ3" s="0"/>
+      <c r="AIR3" s="0"/>
+      <c r="AIS3" s="0"/>
+      <c r="AIT3" s="0"/>
+      <c r="AIU3" s="0"/>
+      <c r="AIV3" s="0"/>
+      <c r="AIW3" s="0"/>
+      <c r="AIX3" s="0"/>
+      <c r="AIY3" s="0"/>
+      <c r="AIZ3" s="0"/>
+      <c r="AJA3" s="0"/>
+      <c r="AJB3" s="0"/>
+      <c r="AJC3" s="0"/>
+      <c r="AJD3" s="0"/>
+      <c r="AJE3" s="0"/>
+      <c r="AJF3" s="0"/>
+      <c r="AJG3" s="0"/>
+      <c r="AJH3" s="0"/>
+      <c r="AJI3" s="0"/>
+      <c r="AJJ3" s="0"/>
+      <c r="AJK3" s="0"/>
+      <c r="AJL3" s="0"/>
+      <c r="AJM3" s="0"/>
+      <c r="AJN3" s="0"/>
+      <c r="AJO3" s="0"/>
+      <c r="AJP3" s="0"/>
+      <c r="AJQ3" s="0"/>
+      <c r="AJR3" s="0"/>
+      <c r="AJS3" s="0"/>
+      <c r="AJT3" s="0"/>
+      <c r="AJU3" s="0"/>
+      <c r="AJV3" s="0"/>
+      <c r="AJW3" s="0"/>
+      <c r="AJX3" s="0"/>
+      <c r="AJY3" s="0"/>
+      <c r="AJZ3" s="0"/>
+      <c r="AKA3" s="0"/>
+      <c r="AKB3" s="0"/>
+      <c r="AKC3" s="0"/>
+      <c r="AKD3" s="0"/>
+      <c r="AKE3" s="0"/>
+      <c r="AKF3" s="0"/>
+      <c r="AKG3" s="0"/>
+      <c r="AKH3" s="0"/>
+      <c r="AKI3" s="0"/>
+      <c r="AKJ3" s="0"/>
+      <c r="AKK3" s="0"/>
+      <c r="AKL3" s="0"/>
+      <c r="AKM3" s="0"/>
+      <c r="AKN3" s="0"/>
+      <c r="AKO3" s="0"/>
+      <c r="AKP3" s="0"/>
+      <c r="AKQ3" s="0"/>
+      <c r="AKR3" s="0"/>
+      <c r="AKS3" s="0"/>
+      <c r="AKT3" s="0"/>
+      <c r="AKU3" s="0"/>
+      <c r="AKV3" s="0"/>
+      <c r="AKW3" s="0"/>
+      <c r="AKX3" s="0"/>
+      <c r="AKY3" s="0"/>
+      <c r="AKZ3" s="0"/>
+      <c r="ALA3" s="0"/>
+      <c r="ALB3" s="0"/>
+      <c r="ALC3" s="0"/>
+      <c r="ALD3" s="0"/>
+      <c r="ALE3" s="0"/>
+      <c r="ALF3" s="0"/>
+      <c r="ALG3" s="0"/>
+      <c r="ALH3" s="0"/>
+      <c r="ALI3" s="0"/>
+      <c r="ALJ3" s="0"/>
+      <c r="ALK3" s="0"/>
+      <c r="ALL3" s="0"/>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F10" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F14" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F17" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F18" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F19" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F20" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F21" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F23" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F24" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F25" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M25" s="4"/>
-      <c r="N25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F26" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M26" s="4"/>
-      <c r="N26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>27</v>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3942,244 +4184,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:26 A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>